<commit_message>
Add typing for excel processing
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>name</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>power_2ohm</t>
+  </si>
+  <si>
+    <t>"9001"</t>
   </si>
 </sst>
 </file>
@@ -602,7 +605,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,8 +687,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>9001</v>
+      <c r="A4" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -864,7 +867,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Black formatting and WIP on front
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ewael\Documents\Unisson\LimiterRMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tberlioz\LimiterRMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4F2FE1-98D5-4678-983A-16B3742AC020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="11700"/>
+    <workbookView xWindow="5160" yWindow="2175" windowWidth="17085" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="amplifiers" sheetId="1" r:id="rId1"/>
     <sheet name="speakers" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">amplifiers!$A$1:$G$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">speakers!$A$1:$F$17</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
   <si>
     <t>name</t>
   </si>
@@ -45,9 +50,6 @@
     <t>t.amp TSA 4-1300</t>
   </si>
   <si>
-    <t>TPA</t>
-  </si>
-  <si>
     <t>TPA FP14000</t>
   </si>
   <si>
@@ -87,18 +89,6 @@
     <t>Crest Audio 7001</t>
   </si>
   <si>
-    <t>RMX</t>
-  </si>
-  <si>
-    <t>QSC RMX 1450</t>
-  </si>
-  <si>
-    <t>MDM</t>
-  </si>
-  <si>
-    <t>MDM 1600×4</t>
-  </si>
-  <si>
     <t>response</t>
   </si>
   <si>
@@ -165,9 +155,6 @@
     <t>NEXOH</t>
   </si>
   <si>
-    <t>Nexo Si1000 high</t>
-  </si>
-  <si>
     <t>800-18k</t>
   </si>
   <si>
@@ -271,12 +258,18 @@
   </si>
   <si>
     <t>"9001"</t>
+  </si>
+  <si>
+    <t>Nexo SI1000 high</t>
+  </si>
+  <si>
+    <t>FP14000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -601,23 +594,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="14.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -631,90 +624,87 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
-        <v>37.799999999999997</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1">
-        <v>1220</v>
+        <v>2350</v>
       </c>
       <c r="E2" s="1">
-        <v>1670</v>
+        <v>4400</v>
+      </c>
+      <c r="F2" s="1">
+        <v>7000</v>
       </c>
       <c r="G2" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>35</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="D3" s="1">
-        <v>2350</v>
+        <v>1220</v>
       </c>
       <c r="E3" s="1">
-        <v>4400</v>
-      </c>
-      <c r="F3" s="1">
-        <v>7000</v>
+        <v>1670</v>
       </c>
       <c r="G3" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1">
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="E4" s="1">
-        <v>2050</v>
-      </c>
-      <c r="F4" s="1">
-        <v>3000</v>
+        <v>1700</v>
       </c>
       <c r="G4" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>32</v>
@@ -734,10 +724,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>36</v>
@@ -757,39 +747,45 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>40</v>
       </c>
       <c r="D7" s="1">
-        <v>295</v>
+        <v>1100</v>
       </c>
       <c r="E7" s="1">
-        <v>450</v>
+        <v>2050</v>
       </c>
       <c r="F7" s="1">
-        <v>585</v>
+        <v>3000</v>
       </c>
       <c r="G7" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
+      <c r="A8" s="1">
+        <v>7001</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C8" s="1">
+        <v>40</v>
       </c>
       <c r="D8" s="1">
-        <v>310</v>
+        <v>550</v>
       </c>
       <c r="E8" s="1">
-        <v>480</v>
+        <v>715</v>
       </c>
       <c r="F8" s="1">
-        <v>675</v>
+        <v>850</v>
       </c>
       <c r="G8" s="1">
         <v>2</v>
@@ -797,77 +793,69 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="C9" s="1">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1">
+        <v>310</v>
+      </c>
+      <c r="E9" s="1">
+        <v>480</v>
+      </c>
+      <c r="F9" s="1">
+        <v>675</v>
       </c>
       <c r="G9" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>7001</v>
+      <c r="A10" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1">
-        <v>550</v>
+        <v>295</v>
       </c>
       <c r="E10" s="1">
-        <v>715</v>
+        <v>450</v>
       </c>
       <c r="F10" s="1">
-        <v>850</v>
+        <v>585</v>
       </c>
       <c r="G10" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1600</v>
-      </c>
-      <c r="E12" s="1">
-        <v>2650</v>
-      </c>
-      <c r="F12" s="1">
-        <v>3950</v>
-      </c>
-      <c r="G12" s="1">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:G13" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
+      <sortCondition descending="1" ref="D1:D13"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
+    <sortCondition ref="A1:A12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,24 +879,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1">
         <v>8</v>
@@ -917,18 +905,18 @@
         <v>1500</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1">
         <v>4</v>
@@ -937,18 +925,18 @@
         <v>2000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1">
         <v>4</v>
@@ -957,18 +945,18 @@
         <v>900</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -977,18 +965,18 @@
         <v>1000</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -997,18 +985,18 @@
         <v>600</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1">
         <v>8</v>
@@ -1017,18 +1005,18 @@
         <v>350</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1">
         <v>8</v>
@@ -1037,18 +1025,18 @@
         <v>150</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
@@ -1057,18 +1045,18 @@
         <v>1000</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1">
         <v>8</v>
@@ -1077,18 +1065,18 @@
         <v>500</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1">
         <v>8</v>
@@ -1097,18 +1085,18 @@
         <v>400</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1">
         <v>8</v>
@@ -1117,18 +1105,18 @@
         <v>320</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1">
         <v>8</v>
@@ -1137,18 +1125,18 @@
         <v>700</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C14" s="1">
         <v>8</v>
@@ -1157,18 +1145,18 @@
         <v>300</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1">
         <v>4</v>
@@ -1177,18 +1165,18 @@
         <v>500</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1">
         <v>8</v>
@@ -1197,18 +1185,18 @@
         <v>200</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C17" s="1">
         <v>8</v>
@@ -1217,13 +1205,14 @@
         <v>75</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F17" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove compute button for recap instead
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tberlioz\LimiterRMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F72EDC-2506-4000-AAB2-FD3A9032A953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC739C36-DDAB-436A-BA0E-8D82F4606165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35505" yWindow="2820" windowWidth="17085" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>30-200</t>
   </si>
   <si>
-    <t>Funktion-One F221</t>
-  </si>
-  <si>
     <t>20-200</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>Nexo SI1000 high</t>
+  </si>
+  <si>
+    <t>Funktion One F221</t>
   </si>
 </sst>
 </file>
@@ -545,13 +545,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>13</v>
@@ -742,7 +742,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +776,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
@@ -785,15 +785,15 @@
         <v>1000</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1">
         <v>8</v>
@@ -802,15 +802,15 @@
         <v>320</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
         <v>8</v>
@@ -819,15 +819,15 @@
         <v>500</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1">
         <v>8</v>
@@ -836,15 +836,15 @@
         <v>400</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
@@ -853,15 +853,15 @@
         <v>1000</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1">
         <v>4</v>
@@ -870,15 +870,15 @@
         <v>2000</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1">
         <v>8</v>
@@ -887,15 +887,15 @@
         <v>300</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -904,10 +904,10 @@
         <v>900</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -924,12 +924,12 @@
         <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1">
         <v>8</v>
@@ -938,15 +938,15 @@
         <v>150</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1">
         <v>4</v>
@@ -955,15 +955,15 @@
         <v>600</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1">
         <v>8</v>
@@ -972,15 +972,15 @@
         <v>350</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1">
         <v>8</v>
@@ -989,15 +989,15 @@
         <v>700</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1">
         <v>8</v>
@@ -1006,15 +1006,15 @@
         <v>75</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1">
         <v>4</v>
@@ -1023,15 +1023,15 @@
         <v>500</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1">
         <v>8</v>
@@ -1040,10 +1040,10 @@
         <v>200</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Front layout over now need to do calc
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tberlioz\LimiterRMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ewael\Documents\Unisson\LimiterRMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4F2FE1-98D5-4678-983A-16B3742AC020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="2175" windowWidth="17085" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5160" yWindow="2175" windowWidth="17085" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="amplifiers" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
   <si>
     <t>name</t>
   </si>
@@ -255,9 +254,6 @@
   </si>
   <si>
     <t>power_2ohm</t>
-  </si>
-  <si>
-    <t>"9001"</t>
   </si>
   <si>
     <t>Nexo SI1000 high</t>
@@ -269,7 +265,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -594,11 +590,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,86 +633,92 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>77</v>
+      <c r="A2" s="1">
+        <v>7001</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1">
-        <v>2350</v>
+        <v>550</v>
       </c>
       <c r="E2" s="1">
-        <v>4400</v>
+        <v>715</v>
       </c>
       <c r="F2" s="1">
-        <v>7000</v>
+        <v>850</v>
       </c>
       <c r="G2" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
+      <c r="A3" s="1">
+        <v>9001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>37.799999999999997</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1">
-        <v>1220</v>
+        <v>1100</v>
       </c>
       <c r="E3" s="1">
-        <v>1670</v>
+        <v>2050</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3000</v>
       </c>
       <c r="G3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>35</v>
       </c>
       <c r="D4" s="1">
-        <v>1200</v>
+        <v>2350</v>
       </c>
       <c r="E4" s="1">
-        <v>1700</v>
+        <v>4400</v>
+      </c>
+      <c r="F4" s="1">
+        <v>7000</v>
       </c>
       <c r="G4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1">
         <v>1100</v>
       </c>
       <c r="E5" s="1">
-        <v>1500</v>
+        <v>1800</v>
       </c>
       <c r="F5" s="1">
-        <v>1700</v>
+        <v>2500</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>
@@ -724,22 +726,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1">
         <v>1100</v>
       </c>
       <c r="E6" s="1">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="F6" s="1">
-        <v>2500</v>
+        <v>1700</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -747,45 +749,42 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1">
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="E7" s="1">
-        <v>2050</v>
-      </c>
-      <c r="F7" s="1">
-        <v>3000</v>
+        <v>1700</v>
       </c>
       <c r="G7" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7001</v>
+      <c r="A8" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1">
-        <v>550</v>
+        <v>310</v>
       </c>
       <c r="E8" s="1">
-        <v>715</v>
+        <v>480</v>
       </c>
       <c r="F8" s="1">
-        <v>850</v>
+        <v>675</v>
       </c>
       <c r="G8" s="1">
         <v>2</v>
@@ -793,22 +792,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1">
         <v>26</v>
       </c>
       <c r="D9" s="1">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="E9" s="1">
-        <v>480</v>
+        <v>450</v>
       </c>
       <c r="F9" s="1">
-        <v>675</v>
+        <v>585</v>
       </c>
       <c r="G9" s="1">
         <v>2</v>
@@ -816,34 +815,31 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
-        <v>26</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="D10" s="1">
-        <v>295</v>
+        <v>1220</v>
       </c>
       <c r="E10" s="1">
-        <v>450</v>
-      </c>
-      <c r="F10" s="1">
-        <v>585</v>
+        <v>1670</v>
       </c>
       <c r="G10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G13" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
-      <sortCondition descending="1" ref="D1:D13"/>
+  <autoFilter ref="A1:G13">
+    <sortState ref="A2:G10">
+      <sortCondition ref="A1:A13"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
+  <sortState ref="A2:G12">
     <sortCondition ref="A1:A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -851,11 +847,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,19 +889,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>69</v>
@@ -913,19 +909,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1">
-        <v>2000</v>
+        <v>320</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>69</v>
@@ -933,39 +929,39 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>69</v>
@@ -973,19 +969,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
       </c>
       <c r="D6" s="1">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>70</v>
@@ -993,19 +989,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
-        <v>350</v>
+        <v>2000</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>69</v>
@@ -1013,19 +1009,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C8" s="1">
         <v>8</v>
       </c>
       <c r="D8" s="1">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>69</v>
@@ -1033,59 +1029,59 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1">
         <v>8</v>
       </c>
       <c r="D10" s="1">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1">
         <v>8</v>
       </c>
       <c r="D11" s="1">
-        <v>400</v>
+        <v>150</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>69</v>
@@ -1093,39 +1089,39 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1">
-        <v>320</v>
+        <v>600</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1">
         <v>8</v>
       </c>
       <c r="D13" s="1">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>69</v>
@@ -1133,19 +1129,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" s="1">
         <v>8</v>
       </c>
       <c r="D14" s="1">
-        <v>300</v>
+        <v>700</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>69</v>
@@ -1153,19 +1149,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C15" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1">
-        <v>500</v>
+        <v>75</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>69</v>
@@ -1173,19 +1169,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>69</v>
@@ -1193,26 +1189,30 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1">
         <v>8</v>
       </c>
       <c r="D17" s="1">
-        <v>75</v>
+        <v>200</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F17" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:F17">
+    <sortState ref="A2:F17">
+      <sortCondition ref="A1:A17"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>